<commit_message>
added links to GIS data aquisition
</commit_message>
<xml_diff>
--- a/Code/economics_schema_report.xlsx
+++ b/Code/economics_schema_report.xlsx
@@ -5,22 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://selectenergyservices-my.sharepoint.com/personal/rlafferty_selectwater_com/Documents/Select Doc/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\rlafferty\Documents\Select Doc\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_25EDB0A0D320D40D175A3611595ED87656CC1F4B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD592AAB-34ED-40F9-9409-41A2714E8685}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3956E0-FC54-47EA-9A8D-54306A1A7EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="11670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-255" windowWidth="19440" windowHeight="10440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Economic" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Placedwells" sheetId="2" r:id="rId3"/>
+    <sheet name="PWI_wells" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="527">
   <si>
     <t>Name</t>
   </si>
@@ -734,13 +737,880 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>API_UWI</t>
+  </si>
+  <si>
+    <t>API UWI</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>API_UWI_Unformatted</t>
+  </si>
+  <si>
+    <t>API UWI (Unformatted)</t>
+  </si>
+  <si>
+    <t>BE15To1WTINYMEXHistorical_USDPerBBL</t>
+  </si>
+  <si>
+    <t>BE 15:1 WTI NYMEX Hist. ($/bbl)</t>
+  </si>
+  <si>
+    <t>DOUBLE PRECISION</t>
+  </si>
+  <si>
+    <t>BE15To1WTINYMEXHistorical_USDPerMcf</t>
+  </si>
+  <si>
+    <t>BE 15:1 WTI NYMEX Hist. ($/mcf)</t>
+  </si>
+  <si>
+    <t>BE15To1WTINYMEX_USDPerBBL</t>
+  </si>
+  <si>
+    <t>BE 15:1 WTI NYMEX ($/bbl)</t>
+  </si>
+  <si>
+    <t>BE15To1WTINYMEX_USDPerMcf</t>
+  </si>
+  <si>
+    <t>BE 15:1 WTI NYMEX ($/mcf)</t>
+  </si>
+  <si>
+    <t>BE20To1WTINYMEXHistorical_USDPerBBL</t>
+  </si>
+  <si>
+    <t>BE 20:1 WTI NYMEX Hist. ($/bbl)</t>
+  </si>
+  <si>
+    <t>BE20To1WTINYMEXHistorical_USDPerMcf</t>
+  </si>
+  <si>
+    <t>BE 20:1 WTI NYMEX Hist. ($/mcf)</t>
+  </si>
+  <si>
+    <t>BE20To1WTINYMEX_USDPerBBL</t>
+  </si>
+  <si>
+    <t>BE 20:1 WTI NYMEX ($/bbl)</t>
+  </si>
+  <si>
+    <t>BE20To1WTINYMEX_USDPerMcf</t>
+  </si>
+  <si>
+    <t>BE 20:1 WTI NYMEX ($/mcf)</t>
+  </si>
+  <si>
+    <t>BE25To1HHNYMEXHistorical_USDPerMcf</t>
+  </si>
+  <si>
+    <t>BE 25:1 HH NYMEX Hist. ($/mcf)</t>
+  </si>
+  <si>
+    <t>BE25To1WTINYMEXHistorical_USDPerBBL</t>
+  </si>
+  <si>
+    <t>BE 25:1 WTI NYMEX Hist. ($/bbl)</t>
+  </si>
+  <si>
+    <t>BE25To1WTINYMEX_USDPerBBL</t>
+  </si>
+  <si>
+    <t>BE 25:1 WTI NYMEX ($/bbl)</t>
+  </si>
+  <si>
+    <t>BE25To1WTINYMEX_USDPerMcf</t>
+  </si>
+  <si>
+    <t>BE 25:1 WTI NYMEX ($/mcf)</t>
+  </si>
+  <si>
+    <t>CapitalEfficiency_USDPerBOEPerDAY</t>
+  </si>
+  <si>
+    <t>Capital Efficiency ($/boe/day)</t>
+  </si>
+  <si>
+    <t>CompletionCostHistorical_USDMM</t>
+  </si>
+  <si>
+    <t>Completion Cost Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>CompletionCost_USDMM</t>
+  </si>
+  <si>
+    <t>Completion Cost ($MM)</t>
+  </si>
+  <si>
+    <t>DeletedDate</t>
+  </si>
+  <si>
+    <t>Deleted Date</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>DrillingCostHistorical_USDMM</t>
+  </si>
+  <si>
+    <t>Drilling Cost Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>DrillingCost_USDMM</t>
+  </si>
+  <si>
+    <t>Drilling Cost ($MM)</t>
+  </si>
+  <si>
+    <t>EURPP_MBOE</t>
+  </si>
+  <si>
+    <t>EUR/PP (mboe)</t>
+  </si>
+  <si>
+    <t>EURPP_MBOEPer1000FT</t>
+  </si>
+  <si>
+    <t>EUR/PP (mboe/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURPerSectionAnyZone_MBBL</t>
+  </si>
+  <si>
+    <t>EUR/Section Any Zone (mbbl)</t>
+  </si>
+  <si>
+    <t>EURPerSectionAnyZone_MBOE</t>
+  </si>
+  <si>
+    <t>EUR/Section Any Zone (mboe)</t>
+  </si>
+  <si>
+    <t>EURPerSectionSameZone_MBBL</t>
+  </si>
+  <si>
+    <t>EUR/Section Same Zone (mbbl)</t>
+  </si>
+  <si>
+    <t>EURPerSectionSameZone_MBOE</t>
+  </si>
+  <si>
+    <t>EUR/Section Same Zone (mboe)</t>
+  </si>
+  <si>
+    <t>EURWH_BCFE_360</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (bcfe)</t>
+  </si>
+  <si>
+    <t>EURWH_BCFE_360Per1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (bcfe/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURWH_BCF_360</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (bcf)</t>
+  </si>
+  <si>
+    <t>EURWH_BCF_360Per1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (bcf/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURWH_MBBL_360</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (mbbl)</t>
+  </si>
+  <si>
+    <t>EURWH_MBBL_360Per1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (mbbl/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE</t>
+  </si>
+  <si>
+    <t>EUR WH (mboe)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOEPer1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH (mboe/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_120</t>
+  </si>
+  <si>
+    <t>EUR WH 120 (mboe)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_120Per1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH 120 (mboe/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_180</t>
+  </si>
+  <si>
+    <t>EUR WH 180 (mboe)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_180Per1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH 180 (mboe/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_360</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (mboe)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_360PEr1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH 360 (mboe/1,000 ft)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_60</t>
+  </si>
+  <si>
+    <t>EUR WH 60 (mboe)</t>
+  </si>
+  <si>
+    <t>EURWH_MBOE_60Per1000FT</t>
+  </si>
+  <si>
+    <t>EUR WH 60 (mboe/1,000 ft)</t>
+  </si>
+  <si>
+    <t>FindingAndDevelopment_USDPerBOE</t>
+  </si>
+  <si>
+    <t>Finding &amp; Dev. Cost ($/boe)</t>
+  </si>
+  <si>
+    <t>FixedOpex_USDPerWELLPerMONTH</t>
+  </si>
+  <si>
+    <t>Fixed Opex ($/well/month)</t>
+  </si>
+  <si>
+    <t>ForecastWHLiquids_PCT</t>
+  </si>
+  <si>
+    <t>Forecast WH Liquids (%)</t>
+  </si>
+  <si>
+    <t>GAndA_USDPerBOE</t>
+  </si>
+  <si>
+    <t>G&amp;A ($/boe)</t>
+  </si>
+  <si>
+    <t>GasDifferential_PCT</t>
+  </si>
+  <si>
+    <t>Gas Diff. (%)</t>
+  </si>
+  <si>
+    <t>GasDifferential_USDPerMCF</t>
+  </si>
+  <si>
+    <t>Gas Diff. ($/mcf)</t>
+  </si>
+  <si>
+    <t>GasEURPP_PCT</t>
+  </si>
+  <si>
+    <t>Gas EUR/PP (%)</t>
+  </si>
+  <si>
+    <t>GasEURWH_BCF</t>
+  </si>
+  <si>
+    <t>Gas EUR WH (bcf)</t>
+  </si>
+  <si>
+    <t>GasEURWH_BCFPer1000FT</t>
+  </si>
+  <si>
+    <t>Gas EUR WH (bcf/1,000 ft)</t>
+  </si>
+  <si>
+    <t>GasSeveranceTax_PCT</t>
+  </si>
+  <si>
+    <t>Gas Severance Tax (%)</t>
+  </si>
+  <si>
+    <t>GasShrink_PCT</t>
+  </si>
+  <si>
+    <t>Gas Shrink (%)</t>
+  </si>
+  <si>
+    <t>GenericAcreValue10Yr_USD</t>
+  </si>
+  <si>
+    <t>Generic Acre Value 10 Yr ($)</t>
+  </si>
+  <si>
+    <t>GenericDrainage_AC</t>
+  </si>
+  <si>
+    <t>Generic Drainage (ac)</t>
+  </si>
+  <si>
+    <t>HistoricalNPVPerSectionAnyZone</t>
+  </si>
+  <si>
+    <t>Hist. NPV/Section Any Zone</t>
+  </si>
+  <si>
+    <t>HistoricalNPVPerSectionSameZone</t>
+  </si>
+  <si>
+    <t>Hist. NPV/Section Same Zone</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt50And200Historical_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 50&amp;200 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt50And200_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 50&amp;200 ($MM)</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt55And300Historical_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 55&amp;300 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt55And300_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 55&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt60And300Historical_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 60&amp;300 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt60And300_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 60&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt60And350Historical_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 60&amp;350 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>IRRPerWELLAt60And350_USDMM</t>
+  </si>
+  <si>
+    <t>IRR/Well 60&amp;350 ($MM)</t>
+  </si>
+  <si>
+    <t>NGLDifferential_PCT</t>
+  </si>
+  <si>
+    <t>NGL Diff. (%)</t>
+  </si>
+  <si>
+    <t>NGLDifferential_USDPerBBL</t>
+  </si>
+  <si>
+    <t>NGL Diff. ($/bbl)</t>
+  </si>
+  <si>
+    <t>NGLEURPP_PCT</t>
+  </si>
+  <si>
+    <t>NGL EUR/PP (%)</t>
+  </si>
+  <si>
+    <t>NGLSeveranceTax_PCT</t>
+  </si>
+  <si>
+    <t>NGL Severance Tax (%)</t>
+  </si>
+  <si>
+    <t>NGLYield_BBLPerMMCF</t>
+  </si>
+  <si>
+    <t>NGL Yield (bbl/mmcf)</t>
+  </si>
+  <si>
+    <t>NPVPerSectionAnyZone_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Section Any Zone ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerSectionSameZone_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Section Same Zone ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt50And200Historical_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 50&amp;200 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt50And200_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 50&amp;200 ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt55And300Historical_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 55&amp;300 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt55And300_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 55&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt60And300Historical_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 60&amp;300 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt60And300_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 60&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt60And350Historical_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 60&amp;350 Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>NPVPerWELLAt60And350_USDMM</t>
+  </si>
+  <si>
+    <t>NPV/Well 60&amp;350 ($MM)</t>
+  </si>
+  <si>
+    <t>NetbackPerWELLAt50And200_USDMM</t>
+  </si>
+  <si>
+    <t>Netback/Well 50&amp;200 ($MM)</t>
+  </si>
+  <si>
+    <t>NetbackPerWELLAt55And300_USDMM</t>
+  </si>
+  <si>
+    <t>Netback/Well 55&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>NetbackPerWELLAt60And300_USDMM</t>
+  </si>
+  <si>
+    <t>Netback/Well 60&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>NetbackPerWELLAt60And350_USDMM</t>
+  </si>
+  <si>
+    <t>Netback/Well 60&amp;350 ($MM)</t>
+  </si>
+  <si>
+    <t>OilDifferential_PCT</t>
+  </si>
+  <si>
+    <t>Oil Diff. (%)</t>
+  </si>
+  <si>
+    <t>OilDifferential_USDPerBBL</t>
+  </si>
+  <si>
+    <t>Oil Diff. ($/bbl)</t>
+  </si>
+  <si>
+    <t>OilEURPP_PCT</t>
+  </si>
+  <si>
+    <t>Oil EUR/PP (%)</t>
+  </si>
+  <si>
+    <t>OilEURWH_MBBL</t>
+  </si>
+  <si>
+    <t>Oil EUR WH (mbbl)</t>
+  </si>
+  <si>
+    <t>OilEURWH_MBBLPer1000FT</t>
+  </si>
+  <si>
+    <t>Oil EUR WH (mbbl/1,000 ft)</t>
+  </si>
+  <si>
+    <t>OilSeveranceTax_PCT</t>
+  </si>
+  <si>
+    <t>Oil Severance Tax (%)</t>
+  </si>
+  <si>
+    <t>PayoutPeriod_MONTHS</t>
+  </si>
+  <si>
+    <t>Payout Period (months)</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>PostProcessingGrossUp_PCT</t>
+  </si>
+  <si>
+    <t>Post-Processing Gross-Up (%)</t>
+  </si>
+  <si>
+    <t>ProcessingFee_USDPerMCF</t>
+  </si>
+  <si>
+    <t>Processing Fee ($/mcf)</t>
+  </si>
+  <si>
+    <t>RecycleRatioPerWELLAt50And200_USDMM</t>
+  </si>
+  <si>
+    <t>Recycle Ratio/Well 50&amp;200 ($MM)</t>
+  </si>
+  <si>
+    <t>RecycleRatioPerWELLAt55And300_USDMM</t>
+  </si>
+  <si>
+    <t>Recycle Ratio/Well 55&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>RecycleRatioPerWELLAt60And300_USDMM</t>
+  </si>
+  <si>
+    <t>Recycle Ratio/Well 60&amp;300 ($MM)</t>
+  </si>
+  <si>
+    <t>RecycleRatioPerWELLAt60And350_USDMM</t>
+  </si>
+  <si>
+    <t>Recycle Ratio/Well 60&amp;350 ($MM)</t>
+  </si>
+  <si>
+    <t>RoyaltyRateGas_PCT</t>
+  </si>
+  <si>
+    <t>Royalty Rate Gas (%)</t>
+  </si>
+  <si>
+    <t>RoyaltyRateNGL_PCT</t>
+  </si>
+  <si>
+    <t>Royalty Rate NGL (%)</t>
+  </si>
+  <si>
+    <t>RoyaltyRateOil_PCT</t>
+  </si>
+  <si>
+    <t>Royalty Rate Oil (%)</t>
+  </si>
+  <si>
+    <t>TieInCostHistorical_USDMM</t>
+  </si>
+  <si>
+    <t>Tie-In Cost Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>TieInCost_USDMM</t>
+  </si>
+  <si>
+    <t>Tie-In Cost ($MM)</t>
+  </si>
+  <si>
+    <t>TotalOpex_USDPerBOE</t>
+  </si>
+  <si>
+    <t>Total Opex ($/boe)</t>
+  </si>
+  <si>
+    <t>TotalWellCostHistorical_USDMM</t>
+  </si>
+  <si>
+    <t>Total Well Cost Hist. ($MM)</t>
+  </si>
+  <si>
+    <t>TotalWellCost_USDMM</t>
+  </si>
+  <si>
+    <t>Total Well Cost ($MM)</t>
+  </si>
+  <si>
+    <t>TransportationCost_USDPerBOE</t>
+  </si>
+  <si>
+    <t>Transportation Cost ($/boe)</t>
+  </si>
+  <si>
+    <t>UpdatedDate</t>
+  </si>
+  <si>
+    <t>Updated Date</t>
+  </si>
+  <si>
+    <t>VariableOpex_USDPerBOE</t>
+  </si>
+  <si>
+    <t>Variable Opex ($/boe)</t>
+  </si>
+  <si>
+    <t>WellID</t>
+  </si>
+  <si>
+    <t>Well ID</t>
+  </si>
+  <si>
+    <t>BIGINT</t>
+  </si>
+  <si>
+    <t>Data Type (SQL)</t>
+  </si>
+  <si>
+    <t>DSUID</t>
+  </si>
+  <si>
+    <t>TIMESTAMP WITHOUT TIME ZONE</t>
+  </si>
+  <si>
+    <t>ENVBasin</t>
+  </si>
+  <si>
+    <t>Basin</t>
+  </si>
+  <si>
+    <t>ENVCounty</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>ENVInterval</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>ENVPWOperator</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>ENVPWSpacingScenario</t>
+  </si>
+  <si>
+    <t>Spacing Scenario</t>
+  </si>
+  <si>
+    <t>ENVPeerGroup</t>
+  </si>
+  <si>
+    <t>Peer Group</t>
+  </si>
+  <si>
+    <t>ENVPlay</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>ENVRegion</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>ENVSubPlay</t>
+  </si>
+  <si>
+    <t>Sub Play</t>
+  </si>
+  <si>
+    <t>ENVWellStatus</t>
+  </si>
+  <si>
+    <t>Well Status</t>
+  </si>
+  <si>
+    <t>Geom_WKT</t>
+  </si>
+  <si>
+    <t>Geom WKT</t>
+  </si>
+  <si>
+    <t>LateralLength</t>
+  </si>
+  <si>
+    <t>Lateral Length (ft)</t>
+  </si>
+  <si>
+    <t>PWAPIUWI</t>
+  </si>
+  <si>
+    <t>PWAzimuthFromGridNorth</t>
+  </si>
+  <si>
+    <t>Azimuth From Grid North (°)</t>
+  </si>
+  <si>
+    <t>PWCoordinateSource</t>
+  </si>
+  <si>
+    <t>Coordinate Source</t>
+  </si>
+  <si>
+    <t>PWLatitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>PWLongitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>PredictedOperatorSource</t>
+  </si>
+  <si>
+    <t>Predicted Operator Source</t>
+  </si>
+  <si>
+    <t>StateProvince</t>
+  </si>
+  <si>
+    <t>State/Province</t>
+  </si>
+  <si>
+    <t>Trajectory</t>
+  </si>
+  <si>
+    <t>Note: Geodatabase Order follows logical categories and numerical ranges you defined. Let me know if you'd like this formatted into a downloadable CSV, expanded into a schema table format (with ESRI types, nullable, etc.), or an alias table format with descriptions and refined abbreviations.</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>dsuid</t>
+  </si>
+  <si>
+    <t>envbasin</t>
+  </si>
+  <si>
+    <t>envcounty</t>
+  </si>
+  <si>
+    <t>envinterval</t>
+  </si>
+  <si>
+    <t>envpwoperator</t>
+  </si>
+  <si>
+    <t>envpwspacingscenario</t>
+  </si>
+  <si>
+    <t>envpeergroup</t>
+  </si>
+  <si>
+    <t>envplay</t>
+  </si>
+  <si>
+    <t>envregion</t>
+  </si>
+  <si>
+    <t>envsubplay</t>
+  </si>
+  <si>
+    <t>envwellstatus</t>
+  </si>
+  <si>
+    <t>geom_wkt</t>
+  </si>
+  <si>
+    <t>laterallength</t>
+  </si>
+  <si>
+    <t>pwapiuwi</t>
+  </si>
+  <si>
+    <t>pwazimuthfromgridnorth</t>
+  </si>
+  <si>
+    <t>Azimuth From Grid North (Â°)</t>
+  </si>
+  <si>
+    <t>pwcoordinatesource</t>
+  </si>
+  <si>
+    <t>pwlatitude</t>
+  </si>
+  <si>
+    <t>pwlongitude</t>
+  </si>
+  <si>
+    <t>predictedoperatorsource</t>
+  </si>
+  <si>
+    <t>stateprovince</t>
+  </si>
+  <si>
+    <t>trajectory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,6 +1622,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -789,10 +1667,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,6 +1696,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1096,16 +1987,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M110"/>
+  <dimension ref="A1:M226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection sqref="A1:M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1178,8 +2070,8 @@
       <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="M2" s="3">
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1210,8 +2102,8 @@
       <c r="L3" t="s">
         <v>17</v>
       </c>
-      <c r="M3">
-        <v>2</v>
+      <c r="M3" s="3">
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1242,8 +2134,8 @@
       <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="M4">
-        <v>3</v>
+      <c r="M4" s="3">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1274,8 +2166,8 @@
       <c r="L5" t="s">
         <v>17</v>
       </c>
-      <c r="M5">
-        <v>4</v>
+      <c r="M5" s="3">
+        <v>1001</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1306,8 +2198,8 @@
       <c r="L6" t="s">
         <v>17</v>
       </c>
-      <c r="M6">
-        <v>5</v>
+      <c r="M6" s="3">
+        <v>1002</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1338,8 +2230,8 @@
       <c r="L7" t="s">
         <v>17</v>
       </c>
-      <c r="M7">
-        <v>6</v>
+      <c r="M7" s="3">
+        <v>1003</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1370,8 +2262,8 @@
       <c r="L8" t="s">
         <v>17</v>
       </c>
-      <c r="M8">
-        <v>7</v>
+      <c r="M8" s="3">
+        <v>1004</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1402,8 +2294,8 @@
       <c r="L9" t="s">
         <v>17</v>
       </c>
-      <c r="M9">
-        <v>8</v>
+      <c r="M9" s="3">
+        <v>1005</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1434,8 +2326,8 @@
       <c r="L10" t="s">
         <v>17</v>
       </c>
-      <c r="M10">
-        <v>9</v>
+      <c r="M10" s="3">
+        <v>1006</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1466,8 +2358,8 @@
       <c r="L11" t="s">
         <v>17</v>
       </c>
-      <c r="M11">
-        <v>10</v>
+      <c r="M11" s="3">
+        <v>1007</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1498,8 +2390,8 @@
       <c r="L12" t="s">
         <v>17</v>
       </c>
-      <c r="M12">
-        <v>11</v>
+      <c r="M12" s="3">
+        <v>1008</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1530,8 +2422,8 @@
       <c r="L13" t="s">
         <v>17</v>
       </c>
-      <c r="M13">
-        <v>12</v>
+      <c r="M13" s="3">
+        <v>1009</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1562,8 +2454,8 @@
       <c r="L14" t="s">
         <v>17</v>
       </c>
-      <c r="M14">
-        <v>13</v>
+      <c r="M14" s="3">
+        <v>1010</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1594,8 +2486,8 @@
       <c r="L15" t="s">
         <v>17</v>
       </c>
-      <c r="M15">
-        <v>14</v>
+      <c r="M15" s="3">
+        <v>1011</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1626,8 +2518,8 @@
       <c r="L16" t="s">
         <v>17</v>
       </c>
-      <c r="M16">
-        <v>15</v>
+      <c r="M16" s="3">
+        <v>1012</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1658,8 +2550,8 @@
       <c r="L17" t="s">
         <v>17</v>
       </c>
-      <c r="M17">
-        <v>16</v>
+      <c r="M17" s="3">
+        <v>1013</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1690,8 +2582,8 @@
       <c r="L18" t="s">
         <v>17</v>
       </c>
-      <c r="M18">
-        <v>17</v>
+      <c r="M18" s="3">
+        <v>1014</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1722,8 +2614,8 @@
       <c r="L19" t="s">
         <v>17</v>
       </c>
-      <c r="M19">
-        <v>18</v>
+      <c r="M19" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1754,8 +2646,8 @@
       <c r="L20" t="s">
         <v>17</v>
       </c>
-      <c r="M20">
-        <v>19</v>
+      <c r="M20" s="3">
+        <v>1015</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1786,8 +2678,8 @@
       <c r="L21" t="s">
         <v>17</v>
       </c>
-      <c r="M21">
-        <v>20</v>
+      <c r="M21" s="3">
+        <v>1016</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1818,8 +2710,8 @@
       <c r="L22" t="s">
         <v>17</v>
       </c>
-      <c r="M22">
-        <v>21</v>
+      <c r="M22" s="3">
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1850,8 +2742,8 @@
       <c r="L23" t="s">
         <v>17</v>
       </c>
-      <c r="M23">
-        <v>22</v>
+      <c r="M23" s="3">
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1882,8 +2774,8 @@
       <c r="L24" t="s">
         <v>17</v>
       </c>
-      <c r="M24">
-        <v>23</v>
+      <c r="M24" s="3">
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1914,8 +2806,8 @@
       <c r="L25" t="s">
         <v>17</v>
       </c>
-      <c r="M25">
-        <v>24</v>
+      <c r="M25" s="3">
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1946,8 +2838,8 @@
       <c r="L26" t="s">
         <v>17</v>
       </c>
-      <c r="M26">
-        <v>25</v>
+      <c r="M26" s="3">
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1978,8 +2870,8 @@
       <c r="L27" t="s">
         <v>17</v>
       </c>
-      <c r="M27">
-        <v>26</v>
+      <c r="M27" s="3">
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2010,8 +2902,8 @@
       <c r="L28" t="s">
         <v>17</v>
       </c>
-      <c r="M28">
-        <v>27</v>
+      <c r="M28" s="3">
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2042,8 +2934,8 @@
       <c r="L29" t="s">
         <v>17</v>
       </c>
-      <c r="M29">
-        <v>28</v>
+      <c r="M29" s="3">
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2074,8 +2966,8 @@
       <c r="L30" t="s">
         <v>17</v>
       </c>
-      <c r="M30">
-        <v>29</v>
+      <c r="M30" s="3">
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2106,8 +2998,8 @@
       <c r="L31" t="s">
         <v>17</v>
       </c>
-      <c r="M31">
-        <v>30</v>
+      <c r="M31" s="3">
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2138,8 +3030,8 @@
       <c r="L32" t="s">
         <v>17</v>
       </c>
-      <c r="M32">
-        <v>31</v>
+      <c r="M32" s="3">
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2170,8 +3062,8 @@
       <c r="L33" t="s">
         <v>17</v>
       </c>
-      <c r="M33">
-        <v>32</v>
+      <c r="M33" s="3">
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2202,8 +3094,8 @@
       <c r="L34" t="s">
         <v>17</v>
       </c>
-      <c r="M34">
-        <v>33</v>
+      <c r="M34" s="3">
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2234,8 +3126,8 @@
       <c r="L35" t="s">
         <v>17</v>
       </c>
-      <c r="M35">
-        <v>34</v>
+      <c r="M35" s="3">
+        <v>313</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2266,8 +3158,8 @@
       <c r="L36" t="s">
         <v>17</v>
       </c>
-      <c r="M36">
-        <v>35</v>
+      <c r="M36" s="3">
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2298,8 +3190,8 @@
       <c r="L37" t="s">
         <v>17</v>
       </c>
-      <c r="M37">
-        <v>36</v>
+      <c r="M37" s="3">
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2330,8 +3222,8 @@
       <c r="L38" t="s">
         <v>17</v>
       </c>
-      <c r="M38">
-        <v>37</v>
+      <c r="M38" s="3">
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2362,8 +3254,8 @@
       <c r="L39" t="s">
         <v>17</v>
       </c>
-      <c r="M39">
-        <v>38</v>
+      <c r="M39" s="3">
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2394,8 +3286,8 @@
       <c r="L40" t="s">
         <v>17</v>
       </c>
-      <c r="M40">
-        <v>39</v>
+      <c r="M40" s="3">
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2426,8 +3318,8 @@
       <c r="L41" t="s">
         <v>17</v>
       </c>
-      <c r="M41">
-        <v>40</v>
+      <c r="M41" s="3">
+        <v>319</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2458,8 +3350,8 @@
       <c r="L42" t="s">
         <v>17</v>
       </c>
-      <c r="M42">
-        <v>41</v>
+      <c r="M42" s="3">
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2490,8 +3382,8 @@
       <c r="L43" t="s">
         <v>17</v>
       </c>
-      <c r="M43">
-        <v>42</v>
+      <c r="M43" s="3">
+        <v>321</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2522,8 +3414,8 @@
       <c r="L44" t="s">
         <v>17</v>
       </c>
-      <c r="M44">
-        <v>43</v>
+      <c r="M44" s="3">
+        <v>1017</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2554,8 +3446,8 @@
       <c r="L45" t="s">
         <v>17</v>
       </c>
-      <c r="M45">
-        <v>44</v>
+      <c r="M45" s="3">
+        <v>1018</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2586,8 +3478,8 @@
       <c r="L46" t="s">
         <v>17</v>
       </c>
-      <c r="M46">
-        <v>45</v>
+      <c r="M46" s="3">
+        <v>1019</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2618,8 +3510,8 @@
       <c r="L47" t="s">
         <v>17</v>
       </c>
-      <c r="M47">
-        <v>46</v>
+      <c r="M47" s="3">
+        <v>1020</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2650,8 +3542,8 @@
       <c r="L48" t="s">
         <v>17</v>
       </c>
-      <c r="M48">
-        <v>47</v>
+      <c r="M48" s="3">
+        <v>1021</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2682,8 +3574,8 @@
       <c r="L49" t="s">
         <v>17</v>
       </c>
-      <c r="M49">
-        <v>48</v>
+      <c r="M49" s="3">
+        <v>1022</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2714,8 +3606,8 @@
       <c r="L50" t="s">
         <v>17</v>
       </c>
-      <c r="M50">
-        <v>49</v>
+      <c r="M50" s="3">
+        <v>1023</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2746,8 +3638,8 @@
       <c r="L51" t="s">
         <v>17</v>
       </c>
-      <c r="M51">
-        <v>50</v>
+      <c r="M51" s="3">
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2778,8 +3670,8 @@
       <c r="L52" t="s">
         <v>17</v>
       </c>
-      <c r="M52">
-        <v>51</v>
+      <c r="M52" s="3">
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -2810,8 +3702,8 @@
       <c r="L53" t="s">
         <v>17</v>
       </c>
-      <c r="M53">
-        <v>52</v>
+      <c r="M53" s="3">
+        <v>1024</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2842,8 +3734,8 @@
       <c r="L54" t="s">
         <v>17</v>
       </c>
-      <c r="M54">
-        <v>53</v>
+      <c r="M54" s="3">
+        <v>1025</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -2874,8 +3766,8 @@
       <c r="L55" t="s">
         <v>17</v>
       </c>
-      <c r="M55">
-        <v>54</v>
+      <c r="M55" s="3">
+        <v>1026</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -2906,8 +3798,8 @@
       <c r="L56" t="s">
         <v>17</v>
       </c>
-      <c r="M56">
-        <v>55</v>
+      <c r="M56" s="3">
+        <v>1027</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -2938,8 +3830,8 @@
       <c r="L57" t="s">
         <v>17</v>
       </c>
-      <c r="M57">
-        <v>56</v>
+      <c r="M57" s="3">
+        <v>1028</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -2970,8 +3862,8 @@
       <c r="L58" t="s">
         <v>17</v>
       </c>
-      <c r="M58">
-        <v>57</v>
+      <c r="M58" s="3">
+        <v>1029</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -3002,8 +3894,8 @@
       <c r="L59" t="s">
         <v>17</v>
       </c>
-      <c r="M59">
-        <v>58</v>
+      <c r="M59" s="3">
+        <v>1030</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3034,8 +3926,8 @@
       <c r="L60" t="s">
         <v>17</v>
       </c>
-      <c r="M60">
-        <v>59</v>
+      <c r="M60" s="3">
+        <v>1031</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3066,8 +3958,8 @@
       <c r="L61" t="s">
         <v>17</v>
       </c>
-      <c r="M61">
-        <v>60</v>
+      <c r="M61" s="3">
+        <v>1032</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3098,8 +3990,8 @@
       <c r="L62" t="s">
         <v>17</v>
       </c>
-      <c r="M62">
-        <v>61</v>
+      <c r="M62" s="3">
+        <v>1033</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3130,8 +4022,8 @@
       <c r="L63" t="s">
         <v>17</v>
       </c>
-      <c r="M63">
-        <v>62</v>
+      <c r="M63" s="3">
+        <v>1034</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3162,8 +4054,8 @@
       <c r="L64" t="s">
         <v>17</v>
       </c>
-      <c r="M64">
-        <v>63</v>
+      <c r="M64" s="3">
+        <v>1035</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -3194,8 +4086,8 @@
       <c r="L65" t="s">
         <v>17</v>
       </c>
-      <c r="M65">
-        <v>64</v>
+      <c r="M65" s="3">
+        <v>1036</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -3226,8 +4118,8 @@
       <c r="L66" t="s">
         <v>17</v>
       </c>
-      <c r="M66">
-        <v>65</v>
+      <c r="M66" s="3">
+        <v>1037</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3258,8 +4150,8 @@
       <c r="L67" t="s">
         <v>17</v>
       </c>
-      <c r="M67">
-        <v>66</v>
+      <c r="M67" s="3">
+        <v>1038</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -3290,8 +4182,8 @@
       <c r="L68" t="s">
         <v>17</v>
       </c>
-      <c r="M68">
-        <v>67</v>
+      <c r="M68" s="3">
+        <v>1039</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3322,8 +4214,8 @@
       <c r="L69" t="s">
         <v>17</v>
       </c>
-      <c r="M69">
-        <v>68</v>
+      <c r="M69" s="3">
+        <v>1040</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -3354,8 +4246,8 @@
       <c r="L70" t="s">
         <v>17</v>
       </c>
-      <c r="M70">
-        <v>69</v>
+      <c r="M70" s="3">
+        <v>1041</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -3386,8 +4278,8 @@
       <c r="L71" t="s">
         <v>17</v>
       </c>
-      <c r="M71">
-        <v>70</v>
+      <c r="M71" s="3">
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3418,8 +4310,8 @@
       <c r="L72" t="s">
         <v>17</v>
       </c>
-      <c r="M72">
-        <v>71</v>
+      <c r="M72" s="3">
+        <v>1042</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -3450,8 +4342,8 @@
       <c r="L73" t="s">
         <v>17</v>
       </c>
-      <c r="M73">
-        <v>72</v>
+      <c r="M73" s="3">
+        <v>1043</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -3482,8 +4374,8 @@
       <c r="L74" t="s">
         <v>17</v>
       </c>
-      <c r="M74">
-        <v>73</v>
+      <c r="M74" s="3">
+        <v>1044</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -3514,8 +4406,8 @@
       <c r="L75" t="s">
         <v>17</v>
       </c>
-      <c r="M75">
-        <v>74</v>
+      <c r="M75" s="3">
+        <v>1045</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -3546,8 +4438,8 @@
       <c r="L76" t="s">
         <v>17</v>
       </c>
-      <c r="M76">
-        <v>75</v>
+      <c r="M76" s="3">
+        <v>1046</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -3578,8 +4470,8 @@
       <c r="L77" t="s">
         <v>17</v>
       </c>
-      <c r="M77">
-        <v>76</v>
+      <c r="M77" s="3">
+        <v>1047</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -3610,8 +4502,8 @@
       <c r="L78" t="s">
         <v>17</v>
       </c>
-      <c r="M78">
-        <v>77</v>
+      <c r="M78" s="3">
+        <v>1048</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -3642,8 +4534,8 @@
       <c r="L79" t="s">
         <v>17</v>
       </c>
-      <c r="M79">
-        <v>78</v>
+      <c r="M79" s="3">
+        <v>1049</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -3674,8 +4566,8 @@
       <c r="L80" t="s">
         <v>17</v>
       </c>
-      <c r="M80">
-        <v>79</v>
+      <c r="M80" s="3">
+        <v>1050</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -3706,8 +4598,8 @@
       <c r="L81" t="s">
         <v>17</v>
       </c>
-      <c r="M81">
-        <v>80</v>
+      <c r="M81" s="3">
+        <v>1051</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -3738,8 +4630,8 @@
       <c r="L82" t="s">
         <v>17</v>
       </c>
-      <c r="M82">
-        <v>81</v>
+      <c r="M82" s="3">
+        <v>1052</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -3770,8 +4662,8 @@
       <c r="L83" t="s">
         <v>17</v>
       </c>
-      <c r="M83">
-        <v>82</v>
+      <c r="M83" s="3">
+        <v>1053</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -3802,8 +4694,8 @@
       <c r="L84" t="s">
         <v>17</v>
       </c>
-      <c r="M84">
-        <v>83</v>
+      <c r="M84" s="3">
+        <v>1054</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -3834,8 +4726,8 @@
       <c r="L85" t="s">
         <v>17</v>
       </c>
-      <c r="M85">
-        <v>84</v>
+      <c r="M85" s="3">
+        <v>1055</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -3866,8 +4758,8 @@
       <c r="L86" t="s">
         <v>17</v>
       </c>
-      <c r="M86">
-        <v>85</v>
+      <c r="M86" s="3">
+        <v>1056</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -3898,8 +4790,8 @@
       <c r="L87" t="s">
         <v>17</v>
       </c>
-      <c r="M87">
-        <v>86</v>
+      <c r="M87" s="3">
+        <v>1057</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -3930,8 +4822,8 @@
       <c r="L88" t="s">
         <v>17</v>
       </c>
-      <c r="M88">
-        <v>87</v>
+      <c r="M88" s="3">
+        <v>1058</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -3962,8 +4854,8 @@
       <c r="L89" t="s">
         <v>17</v>
       </c>
-      <c r="M89">
-        <v>88</v>
+      <c r="M89" s="3">
+        <v>325</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -3994,8 +4886,8 @@
       <c r="L90" t="s">
         <v>17</v>
       </c>
-      <c r="M90">
-        <v>89</v>
+      <c r="M90" s="3">
+        <v>326</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -4026,8 +4918,8 @@
       <c r="L91" t="s">
         <v>17</v>
       </c>
-      <c r="M91">
-        <v>90</v>
+      <c r="M91" s="3">
+        <v>1059</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -4058,8 +4950,8 @@
       <c r="L92" t="s">
         <v>17</v>
       </c>
-      <c r="M92">
-        <v>91</v>
+      <c r="M92" s="3">
+        <v>1060</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -4090,8 +4982,8 @@
       <c r="L93" t="s">
         <v>17</v>
       </c>
-      <c r="M93">
-        <v>92</v>
+      <c r="M93" s="3">
+        <v>1061</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -4122,8 +5014,8 @@
       <c r="L94" t="s">
         <v>17</v>
       </c>
-      <c r="M94">
-        <v>93</v>
+      <c r="M94" s="3">
+        <v>1062</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -4154,8 +5046,8 @@
       <c r="L95" t="s">
         <v>17</v>
       </c>
-      <c r="M95">
-        <v>94</v>
+      <c r="M95" s="3">
+        <v>1063</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4186,8 +5078,8 @@
       <c r="L96" t="s">
         <v>17</v>
       </c>
-      <c r="M96">
-        <v>95</v>
+      <c r="M96" s="3">
+        <v>1064</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -4218,8 +5110,8 @@
       <c r="L97" t="s">
         <v>17</v>
       </c>
-      <c r="M97">
-        <v>96</v>
+      <c r="M97" s="3">
+        <v>1065</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4250,8 +5142,8 @@
       <c r="L98" t="s">
         <v>17</v>
       </c>
-      <c r="M98">
-        <v>97</v>
+      <c r="M98" s="3">
+        <v>1066</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4282,8 +5174,8 @@
       <c r="L99" t="s">
         <v>17</v>
       </c>
-      <c r="M99">
-        <v>98</v>
+      <c r="M99" s="3">
+        <v>1067</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4314,8 +5206,8 @@
       <c r="L100" t="s">
         <v>17</v>
       </c>
-      <c r="M100">
-        <v>99</v>
+      <c r="M100" s="3">
+        <v>1068</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4346,8 +5238,8 @@
       <c r="L101" t="s">
         <v>17</v>
       </c>
-      <c r="M101">
-        <v>100</v>
+      <c r="M101" s="3">
+        <v>1069</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4378,8 +5270,8 @@
       <c r="L102" t="s">
         <v>17</v>
       </c>
-      <c r="M102">
-        <v>101</v>
+      <c r="M102" s="3">
+        <v>1070</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4410,8 +5302,8 @@
       <c r="L103" t="s">
         <v>17</v>
       </c>
-      <c r="M103">
-        <v>102</v>
+      <c r="M103" s="3">
+        <v>1071</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4442,8 +5334,8 @@
       <c r="L104" t="s">
         <v>17</v>
       </c>
-      <c r="M104">
-        <v>103</v>
+      <c r="M104" s="3">
+        <v>1072</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -4474,8 +5366,8 @@
       <c r="L105" t="s">
         <v>17</v>
       </c>
-      <c r="M105">
-        <v>104</v>
+      <c r="M105" s="3">
+        <v>1073</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -4506,8 +5398,8 @@
       <c r="L106" t="s">
         <v>17</v>
       </c>
-      <c r="M106">
-        <v>105</v>
+      <c r="M106" s="3">
+        <v>1074</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4538,8 +5430,8 @@
       <c r="L107" t="s">
         <v>17</v>
       </c>
-      <c r="M107">
-        <v>106</v>
+      <c r="M107" s="3">
+        <v>1075</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -4570,8 +5462,8 @@
       <c r="L108" t="s">
         <v>17</v>
       </c>
-      <c r="M108">
-        <v>107</v>
+      <c r="M108" s="3">
+        <v>501</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -4602,8 +5494,8 @@
       <c r="L109" t="s">
         <v>17</v>
       </c>
-      <c r="M109">
-        <v>108</v>
+      <c r="M109" s="3">
+        <v>1076</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -4637,11 +5529,2777 @@
       <c r="L110" t="s">
         <v>16</v>
       </c>
-      <c r="M110">
-        <v>109</v>
+      <c r="M110" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D118" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D119" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D120" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D121" s="3">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D122" s="3">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D123" s="3">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D124" s="3">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D125" s="3">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D126" s="3">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D127" s="3">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D128" s="3">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D129" s="3">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D130" s="3">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D131" s="3">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D132" s="3">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D133" s="3">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D134" s="3">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D135" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D136" s="3">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D137" s="3">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D138" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D139" s="3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D140" s="3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D141" s="3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D142" s="3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D143" s="3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D144" s="3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D145" s="3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D146" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D147" s="3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D148" s="3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D149" s="3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D150" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D151" s="3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D152" s="3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D153" s="3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D154" s="3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D155" s="3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D156" s="3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D157" s="3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D158" s="3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D159" s="3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D160" s="3">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D161" s="3">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D162" s="3">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D163" s="3">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D164" s="3">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D165" s="3">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D166" s="3">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D167" s="3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D168" s="3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D169" s="3">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D170" s="3">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D171" s="3">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D172" s="3">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D173" s="3">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D174" s="3">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D175" s="3">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D176" s="3">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D177" s="3">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D178" s="3">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D179" s="3">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D180" s="3">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D181" s="3">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D182" s="3">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D183" s="3">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D184" s="3">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D185" s="3">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D186" s="3">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D187" s="3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D188" s="3">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D189" s="3">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D190" s="3">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D191" s="3">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D192" s="3">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D193" s="3">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D194" s="3">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D195" s="3">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D196" s="3">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D197" s="3">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D198" s="3">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D199" s="3">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D200" s="3">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D201" s="3">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D202" s="3">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A203" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D203" s="3">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D204" s="3">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D205" s="3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D206" s="3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D207" s="3">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D208" s="3">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D209" s="3">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D210" s="3">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D211" s="3">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D212" s="3">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D213" s="3">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D214" s="3">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D215" s="3">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D216" s="3">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D217" s="3">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D218" s="3">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D219" s="3">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D220" s="3">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D221" s="3">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D222" s="3">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D223" s="3">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D224" s="3">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A225" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D225" s="3">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D226" s="3">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA08857-59B6-4FF9-8189-8F31C1F4B931}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB20E7F-4DA9-4A02-8802-772CD20F4C24}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D8" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D17" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D21" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D30" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A7801F-28D5-46DA-A855-D7889300AD40}">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B4" t="s">
+        <v>466</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B5" t="s">
+        <v>468</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>508</v>
+      </c>
+      <c r="B6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>50</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>509</v>
+      </c>
+      <c r="B7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>75</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>510</v>
+      </c>
+      <c r="B8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>511</v>
+      </c>
+      <c r="B9" t="s">
+        <v>476</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>512</v>
+      </c>
+      <c r="B10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>50</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>513</v>
+      </c>
+      <c r="B11" t="s">
+        <v>480</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>514</v>
+      </c>
+      <c r="B12" t="s">
+        <v>482</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>50</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>515</v>
+      </c>
+      <c r="B13" t="s">
+        <v>484</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>30</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>516</v>
+      </c>
+      <c r="B14" t="s">
+        <v>486</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>255</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>517</v>
+      </c>
+      <c r="B15" t="s">
+        <v>488</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>518</v>
+      </c>
+      <c r="B16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>32</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>519</v>
+      </c>
+      <c r="B17" t="s">
+        <v>520</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>18</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>521</v>
+      </c>
+      <c r="B18" t="s">
+        <v>493</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>30</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>522</v>
+      </c>
+      <c r="B19" t="s">
+        <v>495</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>18</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>523</v>
+      </c>
+      <c r="B20" t="s">
+        <v>497</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>524</v>
+      </c>
+      <c r="B21" t="s">
+        <v>499</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>50</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>525</v>
+      </c>
+      <c r="B22" t="s">
+        <v>501</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>30</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>526</v>
+      </c>
+      <c r="B23" t="s">
+        <v>502</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>50</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>231</v>
+      </c>
+      <c r="B24" t="s">
+        <v>232</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C25" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>